<commit_message>
Code changes for Run based
</commit_message>
<xml_diff>
--- a/MasterData/4. AmortTemplateUniversal HD.xlsx
+++ b/MasterData/4. AmortTemplateUniversal HD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7215" tabRatio="643" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7215" tabRatio="643"/>
   </bookViews>
   <sheets>
     <sheet name="AmortTemplateSectionGrid" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="60">
   <si>
     <t>AmortTemplateName</t>
   </si>
@@ -550,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5147,12 +5147,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A110"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5216,7 +5213,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>119</v>
       </c>
@@ -5261,7 +5258,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>119</v>
       </c>
@@ -5347,12 +5344,11 @@
         <f t="shared" si="0"/>
         <v>119Acquired MoviesMoviesAcquired Movies</v>
       </c>
-      <c r="N4" s="2" t="e">
-        <f>VLOOKUP(M4,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N4" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>119</v>
       </c>
@@ -5438,9 +5434,8 @@
         <f t="shared" si="0"/>
         <v>119Acquired MoviesOriginal MiniSeriesAcquired Movies</v>
       </c>
-      <c r="N6" s="2" t="e">
-        <f>VLOOKUP(M6,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N6" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -5484,12 +5479,11 @@
         <f t="shared" si="0"/>
         <v>119Acquired MoviesSeriesAcquired Movies</v>
       </c>
-      <c r="N7" s="2" t="e">
-        <f>VLOOKUP(M7,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>119</v>
       </c>
@@ -5534,7 +5528,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>120</v>
       </c>
@@ -5620,12 +5614,11 @@
         <f t="shared" si="0"/>
         <v>120Acquired SeriesBio/Clip (E)Acquired Series</v>
       </c>
-      <c r="N10" s="2" t="e">
-        <f>VLOOKUP(M10,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>120</v>
       </c>
@@ -5670,7 +5663,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>120</v>
       </c>
@@ -5715,7 +5708,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>120</v>
       </c>
@@ -5763,7 +5756,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>120</v>
       </c>
@@ -5808,7 +5801,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>120</v>
       </c>
@@ -5853,7 +5846,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>120</v>
       </c>
@@ -5939,12 +5932,11 @@
         <f t="shared" si="0"/>
         <v>120Acquired SeriesSeriesAcquired Series</v>
       </c>
-      <c r="N17" s="2" t="e">
-        <f>VLOOKUP(M17,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N17" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>120</v>
       </c>
@@ -5989,7 +5981,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>120</v>
       </c>
@@ -6075,12 +6067,11 @@
         <f t="shared" si="0"/>
         <v>121Acquired MiniSeriesAcquired MiniSeriesAcquired MiniSeries</v>
       </c>
-      <c r="N20" s="2" t="e">
-        <f>VLOOKUP(M20,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>121</v>
       </c>
@@ -6125,7 +6116,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>121</v>
       </c>
@@ -6170,7 +6161,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>122</v>
       </c>
@@ -6215,7 +6206,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>122</v>
       </c>
@@ -6260,7 +6251,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>122</v>
       </c>
@@ -6305,7 +6296,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>122</v>
       </c>
@@ -6350,7 +6341,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>124</v>
       </c>
@@ -6398,7 +6389,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>124</v>
       </c>
@@ -6443,7 +6434,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>124</v>
       </c>
@@ -6488,7 +6479,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>124</v>
       </c>
@@ -6533,7 +6524,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>124</v>
       </c>
@@ -6578,7 +6569,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>125</v>
       </c>
@@ -6623,7 +6614,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>125</v>
       </c>
@@ -6668,7 +6659,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>125</v>
       </c>
@@ -6713,7 +6704,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>125</v>
       </c>
@@ -6758,7 +6749,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>125</v>
       </c>
@@ -6803,7 +6794,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>125</v>
       </c>
@@ -6848,7 +6839,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>125</v>
       </c>
@@ -6893,7 +6884,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>126</v>
       </c>
@@ -6979,12 +6970,11 @@
         <f t="shared" si="0"/>
         <v>127Original SeriesBio/Clip (E)Original Series</v>
       </c>
-      <c r="N40" s="2" t="e">
-        <f>VLOOKUP(M40,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N40" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>127</v>
       </c>
@@ -7073,12 +7063,11 @@
         <f t="shared" si="0"/>
         <v>127Original SeriesDocumentaryOriginal Series</v>
       </c>
-      <c r="N42" s="2" t="e">
-        <f>VLOOKUP(M42,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N42" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>127</v>
       </c>
@@ -7126,7 +7115,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>127</v>
       </c>
@@ -7174,7 +7163,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>127</v>
       </c>
@@ -7222,7 +7211,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>127</v>
       </c>
@@ -7311,9 +7300,8 @@
         <f t="shared" si="0"/>
         <v>127Original SeriesOriginal SeriesOriginal Series</v>
       </c>
-      <c r="N47" s="2" t="e">
-        <f>VLOOKUP(M47,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N47" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
@@ -7357,9 +7345,8 @@
         <f t="shared" si="0"/>
         <v>127Original SeriesPilotOriginal Series</v>
       </c>
-      <c r="N48" s="2" t="e">
-        <f>VLOOKUP(M48,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N48" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -7403,9 +7390,8 @@
         <f t="shared" si="0"/>
         <v>127Original SeriesSeriesOriginal Series</v>
       </c>
-      <c r="N49" s="2" t="e">
-        <f>VLOOKUP(M49,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N49" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -7449,9 +7435,8 @@
         <f t="shared" si="0"/>
         <v>127Original SeriesSpecialOriginal Series</v>
       </c>
-      <c r="N50" s="2" t="e">
-        <f>VLOOKUP(M50,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N50" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -7495,9 +7480,8 @@
         <f t="shared" si="0"/>
         <v>127Original SeriesSportsOriginal Series</v>
       </c>
-      <c r="N51" s="2" t="e">
-        <f>VLOOKUP(M51,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N51" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -7541,12 +7525,11 @@
         <f t="shared" si="0"/>
         <v>127Original SeriesTopicalsOriginal Series</v>
       </c>
-      <c r="N52" s="2" t="e">
-        <f>VLOOKUP(M52,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N52" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>128</v>
       </c>
@@ -7591,7 +7574,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>128</v>
       </c>
@@ -7636,7 +7619,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>128</v>
       </c>
@@ -7681,7 +7664,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>128</v>
       </c>
@@ -7729,7 +7712,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>128</v>
       </c>
@@ -7774,7 +7757,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>128</v>
       </c>
@@ -7819,7 +7802,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>128</v>
       </c>
@@ -7864,7 +7847,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>128</v>
       </c>
@@ -7909,7 +7892,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>128</v>
       </c>
@@ -7954,7 +7937,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>128</v>
       </c>
@@ -7999,7 +7982,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>128</v>
       </c>
@@ -8044,7 +8027,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>128</v>
       </c>
@@ -8089,7 +8072,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>128</v>
       </c>
@@ -8134,7 +8117,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>129</v>
       </c>
@@ -8179,7 +8162,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>129</v>
       </c>
@@ -8224,7 +8207,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>129</v>
       </c>
@@ -8269,7 +8252,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>129</v>
       </c>
@@ -8317,7 +8300,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>129</v>
       </c>
@@ -8362,7 +8345,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>129</v>
       </c>
@@ -8407,7 +8390,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>129</v>
       </c>
@@ -8452,7 +8435,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>129</v>
       </c>
@@ -8497,7 +8480,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>129</v>
       </c>
@@ -8542,7 +8525,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>129</v>
       </c>
@@ -8587,7 +8570,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>129</v>
       </c>
@@ -8632,7 +8615,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>129</v>
       </c>
@@ -8677,7 +8660,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>129</v>
       </c>
@@ -8722,7 +8705,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>130</v>
       </c>
@@ -8767,7 +8750,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>130</v>
       </c>
@@ -8812,7 +8795,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>130</v>
       </c>
@@ -8857,7 +8840,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>130</v>
       </c>
@@ -8902,7 +8885,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>130</v>
       </c>
@@ -8947,7 +8930,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>130</v>
       </c>
@@ -8992,7 +8975,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>130</v>
       </c>
@@ -9037,7 +9020,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>131</v>
       </c>
@@ -9082,7 +9065,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>132</v>
       </c>
@@ -9127,7 +9110,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>132</v>
       </c>
@@ -9172,7 +9155,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>132</v>
       </c>
@@ -9217,7 +9200,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>132</v>
       </c>
@@ -9262,7 +9245,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>133</v>
       </c>
@@ -9307,7 +9290,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>133</v>
       </c>
@@ -9352,7 +9335,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>133</v>
       </c>
@@ -9397,7 +9380,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>133</v>
       </c>
@@ -9445,7 +9428,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>133</v>
       </c>
@@ -9490,7 +9473,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>133</v>
       </c>
@@ -9535,7 +9518,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>133</v>
       </c>
@@ -9580,7 +9563,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>133</v>
       </c>
@@ -9625,7 +9608,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>133</v>
       </c>
@@ -9670,7 +9653,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>133</v>
       </c>
@@ -9715,7 +9698,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>133</v>
       </c>
@@ -9760,7 +9743,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>133</v>
       </c>
@@ -9805,7 +9788,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>133</v>
       </c>
@@ -9891,9 +9874,8 @@
         <f t="shared" si="1"/>
         <v>134PilotDocumentaryOriginal Movies</v>
       </c>
-      <c r="N104" s="2" t="e">
-        <f>VLOOKUP(M104,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N104" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
@@ -9937,9 +9919,8 @@
         <f t="shared" si="1"/>
         <v>134PilotMoviesOriginal Movies</v>
       </c>
-      <c r="N105" s="2" t="e">
-        <f>VLOOKUP(M105,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N105" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="O105" s="2"/>
     </row>
@@ -9984,9 +9965,8 @@
         <f t="shared" si="1"/>
         <v>134PilotOriginalOriginal Movies</v>
       </c>
-      <c r="N106" s="2" t="e">
-        <f>VLOOKUP(M106,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N106" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="O106" s="2"/>
     </row>
@@ -10031,9 +10011,8 @@
         <f t="shared" si="1"/>
         <v>134PilotOriginal MiniSeriesOriginal Movies</v>
       </c>
-      <c r="N107" s="2" t="e">
-        <f>VLOOKUP(M107,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N107" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="O107" s="2"/>
     </row>
@@ -10078,9 +10057,8 @@
         <f t="shared" si="1"/>
         <v>134PilotOriginal SeriesOriginal Movies</v>
       </c>
-      <c r="N108" s="2" t="e">
-        <f>VLOOKUP(M108,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N108" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="O108" s="2"/>
     </row>
@@ -10125,9 +10103,8 @@
         <f t="shared" si="1"/>
         <v>134PilotPilotOriginal Movies</v>
       </c>
-      <c r="N109" s="2" t="e">
-        <f>VLOOKUP(M109,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N109" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="O109" s="2"/>
     </row>
@@ -10172,13 +10149,12 @@
         <f t="shared" si="1"/>
         <v>134PilotSeriesOriginal Movies</v>
       </c>
-      <c r="N110" s="2" t="e">
-        <f>VLOOKUP(M110,Result!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N110" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="O110" s="2"/>
     </row>
-    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>135</v>
       </c>
@@ -10226,7 +10202,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>135</v>
       </c>
@@ -10274,7 +10250,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>135</v>
       </c>
@@ -10322,7 +10298,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>135</v>
       </c>
@@ -10370,7 +10346,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>135</v>
       </c>
@@ -10418,7 +10394,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="116" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>135</v>
       </c>
@@ -10466,7 +10442,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>135</v>
       </c>
@@ -10514,7 +10490,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>135</v>
       </c>
@@ -10562,7 +10538,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>135</v>
       </c>
@@ -10610,7 +10586,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>135</v>
       </c>
@@ -10658,7 +10634,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>135</v>
       </c>
@@ -10706,7 +10682,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="122" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>178</v>
       </c>
@@ -10754,7 +10730,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>178</v>
       </c>
@@ -10802,7 +10778,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>178</v>
       </c>
@@ -10850,7 +10826,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>178</v>
       </c>
@@ -10928,13 +10904,6 @@
       <c r="E133" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O125">
-    <filterColumn colId="13">
-      <filters>
-        <filter val="#N/A"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -10947,8 +10916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:E79"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12618,198 +12587,513 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>134</v>
+      </c>
+      <c r="B80" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" t="s">
+        <v>19</v>
+      </c>
+      <c r="D80" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" t="s">
+        <v>55</v>
+      </c>
       <c r="F80" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
+        <v>134PilotMoviesOriginal Movies</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>134</v>
+      </c>
+      <c r="B81" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" t="s">
+        <v>20</v>
+      </c>
+      <c r="D81" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" t="s">
+        <v>55</v>
+      </c>
       <c r="F81" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
+        <v>134PilotOriginalOriginal Movies</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>134</v>
+      </c>
+      <c r="B82" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" t="s">
+        <v>55</v>
+      </c>
       <c r="F82" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
+        <v>134PilotOriginal SeriesOriginal Movies</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>120</v>
+      </c>
+      <c r="B83" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83" t="s">
+        <v>23</v>
+      </c>
+      <c r="E83" t="s">
+        <v>55</v>
+      </c>
       <c r="F83" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
+        <v>120Acquired SeriesSeriesAcquired Series</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>119</v>
+      </c>
+      <c r="B84" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84" t="s">
+        <v>19</v>
+      </c>
+      <c r="D84" t="s">
+        <v>16</v>
+      </c>
+      <c r="E84" t="s">
+        <v>55</v>
+      </c>
       <c r="F84" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
+        <v>119Acquired MoviesMoviesAcquired Movies</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>134</v>
+      </c>
+      <c r="B85" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" t="s">
+        <v>10</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" t="s">
+        <v>55</v>
+      </c>
       <c r="F85" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
+        <v>134PilotSeriesOriginal Movies</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>121</v>
+      </c>
+      <c r="B86" t="s">
+        <v>17</v>
+      </c>
+      <c r="C86" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86" t="s">
+        <v>17</v>
+      </c>
+      <c r="E86" t="s">
+        <v>55</v>
+      </c>
       <c r="F86" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
+        <v>121Acquired MiniSeriesAcquired MiniSeriesAcquired MiniSeries</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>134</v>
+      </c>
+      <c r="B87" t="s">
+        <v>32</v>
+      </c>
+      <c r="C87" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" t="s">
+        <v>55</v>
+      </c>
       <c r="F87" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
+        <v>134PilotDocumentaryOriginal Movies</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>119</v>
+      </c>
+      <c r="B88" t="s">
+        <v>16</v>
+      </c>
+      <c r="C88" t="s">
+        <v>10</v>
+      </c>
+      <c r="D88" t="s">
+        <v>16</v>
+      </c>
+      <c r="E88" t="s">
+        <v>55</v>
+      </c>
       <c r="F88" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
+        <v>119Acquired MoviesSeriesAcquired Movies</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>120</v>
+      </c>
+      <c r="B89" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" t="s">
+        <v>29</v>
+      </c>
+      <c r="D89" t="s">
+        <v>23</v>
+      </c>
+      <c r="E89" t="s">
+        <v>55</v>
+      </c>
       <c r="F89" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
+        <v>120Acquired SeriesBio/Clip (E)Acquired Series</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>134</v>
+      </c>
+      <c r="B90" t="s">
+        <v>32</v>
+      </c>
+      <c r="C90" t="s">
+        <v>32</v>
+      </c>
+      <c r="D90" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" t="s">
+        <v>55</v>
+      </c>
       <c r="F90" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
+        <v>134PilotPilotOriginal Movies</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>127</v>
+      </c>
+      <c r="B91" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" t="s">
+        <v>33</v>
+      </c>
+      <c r="D91" t="s">
+        <v>15</v>
+      </c>
+      <c r="E91" t="s">
+        <v>55</v>
+      </c>
       <c r="F91" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
+        <v>127Original SeriesTopicalsOriginal Series</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>127</v>
+      </c>
+      <c r="B92" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" t="s">
+        <v>32</v>
+      </c>
+      <c r="D92" t="s">
+        <v>15</v>
+      </c>
+      <c r="E92" t="s">
+        <v>55</v>
+      </c>
       <c r="F92" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="93" spans="6:6" x14ac:dyDescent="0.25">
+        <v>127Original SeriesPilotOriginal Series</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>134</v>
+      </c>
+      <c r="B93" t="s">
+        <v>32</v>
+      </c>
+      <c r="C93" t="s">
+        <v>21</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" t="s">
+        <v>55</v>
+      </c>
       <c r="F93" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="6:6" x14ac:dyDescent="0.25">
+        <v>134PilotOriginal MiniSeriesOriginal Movies</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>119</v>
+      </c>
+      <c r="B94" t="s">
+        <v>16</v>
+      </c>
+      <c r="C94" t="s">
+        <v>21</v>
+      </c>
+      <c r="D94" t="s">
+        <v>16</v>
+      </c>
+      <c r="E94" t="s">
+        <v>55</v>
+      </c>
       <c r="F94" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="95" spans="6:6" x14ac:dyDescent="0.25">
+        <v>119Acquired MoviesOriginal MiniSeriesAcquired Movies</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>127</v>
+      </c>
+      <c r="B95" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" t="s">
+        <v>15</v>
+      </c>
+      <c r="E95" t="s">
+        <v>55</v>
+      </c>
       <c r="F95" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="96" spans="6:6" x14ac:dyDescent="0.25">
+        <v>127Original SeriesBio/Clip (E)Original Series</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>127</v>
+      </c>
+      <c r="B96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C96" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96" t="s">
+        <v>15</v>
+      </c>
+      <c r="E96" t="s">
+        <v>55</v>
+      </c>
       <c r="F96" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
+        <v>127Original SeriesSeriesOriginal Series</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>127</v>
+      </c>
+      <c r="B97" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" t="s">
+        <v>22</v>
+      </c>
+      <c r="D97" t="s">
+        <v>15</v>
+      </c>
+      <c r="E97" t="s">
+        <v>55</v>
+      </c>
       <c r="F97" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
+        <v>127Original SeriesSpecialOriginal Series</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>127</v>
+      </c>
+      <c r="B98" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98" t="s">
+        <v>15</v>
+      </c>
+      <c r="E98" t="s">
+        <v>55</v>
+      </c>
       <c r="F98" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
+        <v>127Original SeriesDocumentaryOriginal Series</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>127</v>
+      </c>
+      <c r="B99" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" t="s">
+        <v>15</v>
+      </c>
+      <c r="D99" t="s">
+        <v>15</v>
+      </c>
+      <c r="E99" t="s">
+        <v>55</v>
+      </c>
       <c r="F99" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
+        <v>127Original SeriesOriginal SeriesOriginal Series</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>127</v>
+      </c>
+      <c r="B100" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" t="s">
+        <v>25</v>
+      </c>
+      <c r="D100" t="s">
+        <v>15</v>
+      </c>
+      <c r="E100" t="s">
+        <v>55</v>
+      </c>
       <c r="F100" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
+        <v>127Original SeriesSportsOriginal Series</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F101" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F102" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F103" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F104" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F105" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F106" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F107" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="108" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F108" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="109" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F109" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="110" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F110" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F111" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="112" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F112" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>

</xml_diff>